<commit_message>
import feature and reports updated
</commit_message>
<xml_diff>
--- a/public/xcelTemplates/CustomersTemplate.xlsx
+++ b/public/xcelTemplates/CustomersTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr.stark/ReactJs Projects/tinatett-pos/public/xcelTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1ABA14-4030-C243-8244-97F48E79C75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C41D86-9402-594F-81FA-3C4286911F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{94BC3CB1-B96D-BB4A-9CF2-2C7A72E9C1E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>CustomerName</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>GD-898-0909</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Ababio and Sons</t>
+  </si>
+  <si>
+    <t>ababioandsons@gmail.com</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>CustomerType</t>
   </si>
 </sst>
 </file>
@@ -428,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF3444D-73FC-4443-A682-5BEC5F3155A8}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,9 +456,10 @@
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="31.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +478,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -478,11 +497,35 @@
       </c>
       <c r="F2" t="s">
         <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>542542299</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{04318A09-49BE-144B-A54D-1D31B7B14179}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{DAEA3E63-760E-F341-8D6A-A2BAE253BBE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>